<commit_message>
updates to match aliases file
</commit_message>
<xml_diff>
--- a/test/registrantExports/SundayEventFilenameDoesNotMatter.xlsx
+++ b/test/registrantExports/SundayEventFilenameDoesNotMatter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sandwich\git\activityAccountant\test\registrantExports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA4E28D-2B52-4C79-8DCE-3D84A71C7DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F9642D-1E79-4245-8D4F-DBCE285EF8A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="296">
   <si>
     <t>ID</t>
   </si>
@@ -403,12 +403,6 @@
     <t>User4</t>
   </si>
   <si>
-    <t>Fake5</t>
-  </si>
-  <si>
-    <t>User5</t>
-  </si>
-  <si>
     <t>Fake6</t>
   </si>
   <si>
@@ -517,18 +511,6 @@
     <t>User23</t>
   </si>
   <si>
-    <t>Fake24</t>
-  </si>
-  <si>
-    <t>User24</t>
-  </si>
-  <si>
-    <t>Fake25</t>
-  </si>
-  <si>
-    <t>User25</t>
-  </si>
-  <si>
     <t>Fake26</t>
   </si>
   <si>
@@ -920,6 +902,12 @@
   </si>
   <si>
     <t>Somerville Curling June-July 2024</t>
+  </si>
+  <si>
+    <t>Multiemail</t>
+  </si>
+  <si>
+    <t>User1Name2</t>
   </si>
 </sst>
 </file>
@@ -1308,14 +1296,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.34765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44921875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.59765625" customWidth="1"/>
     <col min="16" max="16" width="27.09765625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="22.75" bestFit="1" customWidth="1"/>
@@ -1416,7 +1405,7 @@
         <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>29</v>
@@ -1434,7 +1423,7 @@
         <v>1234567890</v>
       </c>
       <c r="P2" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="S2" s="1">
         <v>1</v>
@@ -1461,7 +1450,7 @@
         <v>32</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>33</v>
@@ -1475,7 +1464,7 @@
         <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>29</v>
@@ -1493,7 +1482,7 @@
         <v>1234567891</v>
       </c>
       <c r="P3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="S3" s="1">
         <v>1</v>
@@ -1520,7 +1509,7 @@
         <v>32</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>33</v>
@@ -1534,7 +1523,7 @@
         <v>47</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>29</v>
@@ -1552,7 +1541,7 @@
         <v>1234567892</v>
       </c>
       <c r="P4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="S4" s="1">
         <v>1</v>
@@ -1579,7 +1568,7 @@
         <v>32</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>33</v>
@@ -1593,7 +1582,7 @@
         <v>47</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>29</v>
@@ -1611,7 +1600,7 @@
         <v>1234567893</v>
       </c>
       <c r="P5" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="S5" s="1">
         <v>1</v>
@@ -1638,7 +1627,7 @@
         <v>32</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="AB5" s="1" t="s">
         <v>40</v>
@@ -1652,7 +1641,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>29</v>
@@ -1661,16 +1650,16 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>127</v>
+        <v>294</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="O6" s="1">
         <v>1234567894</v>
       </c>
       <c r="P6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="S6" s="1">
         <v>1</v>
@@ -1697,7 +1686,7 @@
         <v>32</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>33</v>
@@ -1711,7 +1700,7 @@
         <v>47</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>29</v>
@@ -1720,16 +1709,16 @@
         <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O7" s="1">
         <v>1234567895</v>
       </c>
       <c r="P7" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="S7" s="1">
         <v>1</v>
@@ -1756,7 +1745,7 @@
         <v>32</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="AB7" s="1" t="s">
         <v>40</v>
@@ -1770,7 +1759,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>29</v>
@@ -1779,16 +1768,16 @@
         <v>30</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="O8" s="1">
         <v>1234567896</v>
       </c>
       <c r="P8" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="S8" s="1">
         <v>1</v>
@@ -1815,7 +1804,7 @@
         <v>32</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="AB8" s="1" t="s">
         <v>33</v>
@@ -1829,7 +1818,7 @@
         <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>29</v>
@@ -1838,16 +1827,16 @@
         <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="O9" s="1">
         <v>1234567897</v>
       </c>
       <c r="P9" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="S9" s="1">
         <v>1</v>
@@ -1874,7 +1863,7 @@
         <v>32</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="AB9" s="1" t="s">
         <v>33</v>
@@ -1888,7 +1877,7 @@
         <v>47</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>29</v>
@@ -1897,16 +1886,16 @@
         <v>30</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O10" s="1">
         <v>1234567898</v>
       </c>
       <c r="P10" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="S10" s="1">
         <v>1</v>
@@ -1933,7 +1922,7 @@
         <v>32</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="AB10" s="1" t="s">
         <v>33</v>
@@ -1947,7 +1936,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>29</v>
@@ -1956,16 +1945,16 @@
         <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="O11" s="1">
         <v>1234567899</v>
       </c>
       <c r="P11" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="S11" s="1">
         <v>1</v>
@@ -1992,7 +1981,7 @@
         <v>32</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="AB11" s="1" t="s">
         <v>40</v>
@@ -2006,7 +1995,7 @@
         <v>47</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>29</v>
@@ -2015,16 +2004,16 @@
         <v>30</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="O12" s="1">
         <v>1234567900</v>
       </c>
       <c r="P12" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="S12" s="1">
         <v>1</v>
@@ -2051,7 +2040,7 @@
         <v>32</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>40</v>
@@ -2065,7 +2054,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>29</v>
@@ -2074,16 +2063,16 @@
         <v>30</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O13" s="1">
         <v>1234567901</v>
       </c>
       <c r="P13" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="S13" s="1">
         <v>1</v>
@@ -2110,7 +2099,7 @@
         <v>32</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>40</v>
@@ -2124,7 +2113,7 @@
         <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>29</v>
@@ -2133,16 +2122,16 @@
         <v>30</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="O14" s="1">
         <v>1234567902</v>
       </c>
       <c r="P14" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="S14" s="1">
         <v>1</v>
@@ -2169,7 +2158,7 @@
         <v>32</v>
       </c>
       <c r="AA14" s="2" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>40</v>
@@ -2183,7 +2172,7 @@
         <v>47</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>29</v>
@@ -2192,16 +2181,16 @@
         <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="O15" s="1">
         <v>1234567903</v>
       </c>
       <c r="P15" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="S15" s="1">
         <v>1</v>
@@ -2228,7 +2217,7 @@
         <v>32</v>
       </c>
       <c r="AA15" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>33</v>
@@ -2242,7 +2231,7 @@
         <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>29</v>
@@ -2251,16 +2240,16 @@
         <v>30</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="O16" s="1">
         <v>1234567904</v>
       </c>
       <c r="P16" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="S16" s="1">
         <v>1</v>
@@ -2287,7 +2276,7 @@
         <v>32</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>33</v>
@@ -2301,7 +2290,7 @@
         <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>29</v>
@@ -2310,16 +2299,16 @@
         <v>30</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="O17" s="1">
         <v>1234567905</v>
       </c>
       <c r="P17" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="S17" s="1">
         <v>1</v>
@@ -2346,7 +2335,7 @@
         <v>32</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="AB17" s="1" t="s">
         <v>33</v>
@@ -2360,7 +2349,7 @@
         <v>47</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>29</v>
@@ -2369,16 +2358,16 @@
         <v>30</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="O18" s="1">
         <v>1234567906</v>
       </c>
       <c r="P18" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="S18" s="1">
         <v>1</v>
@@ -2405,7 +2394,7 @@
         <v>32</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="AB18" s="1" t="s">
         <v>33</v>
@@ -2419,7 +2408,7 @@
         <v>47</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>29</v>
@@ -2428,16 +2417,16 @@
         <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O19" s="1">
         <v>1234567907</v>
       </c>
       <c r="P19" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="S19" s="1">
         <v>1</v>
@@ -2464,7 +2453,7 @@
         <v>32</v>
       </c>
       <c r="AA19" s="2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>33</v>
@@ -2478,7 +2467,7 @@
         <v>47</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>29</v>
@@ -2487,16 +2476,16 @@
         <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O20" s="1">
         <v>1234567908</v>
       </c>
       <c r="P20" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="S20" s="1">
         <v>1</v>
@@ -2523,7 +2512,7 @@
         <v>32</v>
       </c>
       <c r="AA20" s="2" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="AB20" s="1" t="s">
         <v>33</v>
@@ -2537,7 +2526,7 @@
         <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>29</v>
@@ -2546,16 +2535,16 @@
         <v>30</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="O21" s="1">
         <v>1234567909</v>
       </c>
       <c r="P21" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="S21" s="1">
         <v>1</v>
@@ -2582,7 +2571,7 @@
         <v>32</v>
       </c>
       <c r="AA21" s="2" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="AB21" s="1" t="s">
         <v>33</v>
@@ -2596,7 +2585,7 @@
         <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>29</v>
@@ -2605,16 +2594,16 @@
         <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O22" s="1">
         <v>1234567910</v>
       </c>
       <c r="P22" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="S22" s="1">
         <v>1</v>
@@ -2641,7 +2630,7 @@
         <v>32</v>
       </c>
       <c r="AA22" s="2" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="AB22" s="1" t="s">
         <v>33</v>
@@ -2655,7 +2644,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>29</v>
@@ -2664,16 +2653,16 @@
         <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O23" s="1">
         <v>1234567911</v>
       </c>
       <c r="P23" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="S23" s="1">
         <v>1</v>
@@ -2700,7 +2689,7 @@
         <v>32</v>
       </c>
       <c r="AA23" s="2" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="AB23" s="1" t="s">
         <v>40</v>
@@ -2714,7 +2703,7 @@
         <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>29</v>
@@ -2723,16 +2712,16 @@
         <v>30</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O24" s="1">
         <v>1234567912</v>
       </c>
       <c r="P24" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="S24" s="1">
         <v>1</v>
@@ -2759,7 +2748,7 @@
         <v>32</v>
       </c>
       <c r="AA24" s="2" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>40</v>
@@ -2773,7 +2762,7 @@
         <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>29</v>
@@ -2782,16 +2771,16 @@
         <v>30</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>165</v>
+        <v>294</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>166</v>
+        <v>295</v>
       </c>
       <c r="O25" s="1">
         <v>1234567913</v>
       </c>
       <c r="P25" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="S25" s="1">
         <v>1</v>
@@ -2818,7 +2807,7 @@
         <v>32</v>
       </c>
       <c r="AA25" s="2" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>33</v>
@@ -2832,7 +2821,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>29</v>
@@ -2841,16 +2830,16 @@
         <v>30</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>167</v>
+        <v>294</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>168</v>
+        <v>295</v>
       </c>
       <c r="O26" s="1">
         <v>1234567914</v>
       </c>
       <c r="P26" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="S26" s="1">
         <v>1</v>
@@ -2877,7 +2866,7 @@
         <v>32</v>
       </c>
       <c r="AA26" s="2" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AB26" s="1" t="s">
         <v>33</v>
@@ -2891,7 +2880,7 @@
         <v>47</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>29</v>
@@ -2900,16 +2889,16 @@
         <v>30</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="O27" s="1">
         <v>1234567915</v>
       </c>
       <c r="P27" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="S27" s="1">
         <v>1</v>
@@ -2936,7 +2925,7 @@
         <v>32</v>
       </c>
       <c r="AA27" s="2" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="AB27" s="1" t="s">
         <v>33</v>
@@ -2950,7 +2939,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>29</v>
@@ -2959,16 +2948,16 @@
         <v>30</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="O28" s="1">
         <v>1234567916</v>
       </c>
       <c r="P28" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="S28" s="1">
         <v>1</v>
@@ -2995,7 +2984,7 @@
         <v>32</v>
       </c>
       <c r="AA28" s="2" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="AB28" s="1" t="s">
         <v>33</v>
@@ -3009,7 +2998,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>29</v>
@@ -3018,16 +3007,16 @@
         <v>30</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="O29" s="1">
         <v>1234567917</v>
       </c>
       <c r="P29" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="S29" s="1">
         <v>1</v>
@@ -3054,7 +3043,7 @@
         <v>32</v>
       </c>
       <c r="AA29" s="2" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="AB29" s="1" t="s">
         <v>33</v>
@@ -3068,7 +3057,7 @@
         <v>47</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>29</v>
@@ -3077,16 +3066,16 @@
         <v>30</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="O30" s="1">
         <v>1234567918</v>
       </c>
       <c r="P30" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S30" s="1">
         <v>1</v>
@@ -3113,7 +3102,7 @@
         <v>32</v>
       </c>
       <c r="AA30" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="AB30" s="1" t="s">
         <v>33</v>
@@ -3127,7 +3116,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>29</v>
@@ -3136,16 +3125,16 @@
         <v>30</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="O31" s="1">
         <v>1234567919</v>
       </c>
       <c r="P31" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="S31" s="1">
         <v>1</v>
@@ -3172,7 +3161,7 @@
         <v>32</v>
       </c>
       <c r="AA31" s="2" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="AB31" s="1" t="s">
         <v>33</v>
@@ -3186,7 +3175,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>29</v>
@@ -3195,16 +3184,16 @@
         <v>30</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="O32" s="1">
         <v>1234567920</v>
       </c>
       <c r="P32" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="S32" s="1">
         <v>1</v>
@@ -3231,7 +3220,7 @@
         <v>32</v>
       </c>
       <c r="AA32" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="AB32" s="1" t="s">
         <v>33</v>
@@ -3245,7 +3234,7 @@
         <v>47</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>29</v>
@@ -3254,16 +3243,16 @@
         <v>30</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="O33" s="1">
         <v>1234567921</v>
       </c>
       <c r="P33" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="S33" s="1">
         <v>1</v>
@@ -3290,7 +3279,7 @@
         <v>32</v>
       </c>
       <c r="AA33" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="AB33" s="1" t="s">
         <v>33</v>
@@ -3304,7 +3293,7 @@
         <v>47</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>29</v>
@@ -3314,16 +3303,16 @@
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="O34" s="1">
         <v>1234567922</v>
       </c>
       <c r="P34" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="S34" s="1">
         <v>1</v>
@@ -3350,7 +3339,7 @@
         <v>32</v>
       </c>
       <c r="AA34" s="2" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="AB34" s="1" t="s">
         <v>33</v>
@@ -3364,7 +3353,7 @@
         <v>47</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>29</v>
@@ -3374,16 +3363,16 @@
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="O35" s="1">
         <v>1234567923</v>
       </c>
       <c r="P35" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="S35" s="1">
         <v>1</v>
@@ -3410,7 +3399,7 @@
         <v>32</v>
       </c>
       <c r="AA35" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="AB35" s="1" t="s">
         <v>33</v>
@@ -3424,7 +3413,7 @@
         <v>47</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>29</v>
@@ -3434,16 +3423,16 @@
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="O36" s="1">
         <v>1234567924</v>
       </c>
       <c r="P36" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="S36" s="1">
         <v>1</v>
@@ -3470,7 +3459,7 @@
         <v>32</v>
       </c>
       <c r="AA36" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="AB36" s="1" t="s">
         <v>33</v>
@@ -3484,7 +3473,7 @@
         <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>29</v>
@@ -3494,16 +3483,16 @@
       </c>
       <c r="F37" s="1"/>
       <c r="G37" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="O37" s="1">
         <v>1234567925</v>
       </c>
       <c r="P37" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="S37" s="1">
         <v>1</v>
@@ -3530,7 +3519,7 @@
         <v>32</v>
       </c>
       <c r="AA37" s="2" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="AB37" s="1" t="s">
         <v>33</v>
@@ -3544,7 +3533,7 @@
         <v>47</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>29</v>
@@ -3554,16 +3543,16 @@
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="O38" s="1">
         <v>1234567926</v>
       </c>
       <c r="P38" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="S38" s="1">
         <v>1</v>
@@ -3590,7 +3579,7 @@
         <v>32</v>
       </c>
       <c r="AA38" s="2" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
       <c r="AB38" s="1" t="s">
         <v>33</v>
@@ -3604,7 +3593,7 @@
         <v>47</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>29</v>
@@ -3614,16 +3603,16 @@
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="O39" s="1">
         <v>1234567927</v>
       </c>
       <c r="P39" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="S39" s="1">
         <v>1</v>
@@ -3650,7 +3639,7 @@
         <v>32</v>
       </c>
       <c r="AA39" s="2" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="AB39" s="1" t="s">
         <v>33</v>
@@ -3664,7 +3653,7 @@
         <v>47</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>29</v>
@@ -3673,16 +3662,16 @@
         <v>30</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="O40" s="1">
         <v>1234567928</v>
       </c>
       <c r="P40" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="S40" s="1">
         <v>1</v>
@@ -3709,7 +3698,7 @@
         <v>32</v>
       </c>
       <c r="AA40" s="2" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="AB40" s="1" t="s">
         <v>33</v>
@@ -3723,7 +3712,7 @@
         <v>47</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>29</v>
@@ -3732,16 +3721,16 @@
         <v>30</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="O41" s="1">
         <v>1234567929</v>
       </c>
       <c r="P41" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="S41" s="1">
         <v>1</v>
@@ -3768,7 +3757,7 @@
         <v>32</v>
       </c>
       <c r="AA41" s="2" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="AB41" s="1" t="s">
         <v>33</v>
@@ -3782,7 +3771,7 @@
         <v>47</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>29</v>
@@ -3791,16 +3780,16 @@
         <v>30</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="O42" s="1">
         <v>1234567930</v>
       </c>
       <c r="P42" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="S42" s="1">
         <v>1</v>
@@ -3827,7 +3816,7 @@
         <v>32</v>
       </c>
       <c r="AA42" s="2" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="AB42" s="1" t="s">
         <v>40</v>
@@ -3841,7 +3830,7 @@
         <v>47</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>29</v>
@@ -3850,16 +3839,16 @@
         <v>30</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="O43" s="1">
         <v>1234567931</v>
       </c>
       <c r="P43" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="S43" s="1">
         <v>1</v>
@@ -3886,7 +3875,7 @@
         <v>32</v>
       </c>
       <c r="AA43" s="2" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="AB43" s="1" t="s">
         <v>33</v>
@@ -3900,7 +3889,7 @@
         <v>47</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>29</v>
@@ -3909,16 +3898,16 @@
         <v>30</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="O44" s="1">
         <v>1234567932</v>
       </c>
       <c r="P44" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="S44" s="1">
         <v>1</v>
@@ -3945,7 +3934,7 @@
         <v>32</v>
       </c>
       <c r="AA44" s="2" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="AB44" s="1" t="s">
         <v>33</v>
@@ -3959,7 +3948,7 @@
         <v>47</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>29</v>
@@ -3968,16 +3957,16 @@
         <v>30</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="O45" s="1">
         <v>1234567933</v>
       </c>
       <c r="P45" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="S45" s="1">
         <v>1</v>
@@ -4004,7 +3993,7 @@
         <v>32</v>
       </c>
       <c r="AA45" s="2" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="AB45" s="1" t="s">
         <v>33</v>
@@ -4018,7 +4007,7 @@
         <v>47</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>29</v>
@@ -4027,16 +4016,16 @@
         <v>30</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="O46" s="1">
         <v>1234567934</v>
       </c>
       <c r="P46" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="S46" s="1">
         <v>1</v>
@@ -4063,7 +4052,7 @@
         <v>32</v>
       </c>
       <c r="AA46" s="2" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="AB46" s="1" t="s">
         <v>33</v>

</xml_diff>